<commit_message>
More refinement of area transitions
</commit_message>
<xml_diff>
--- a/Cuisine Quest/Assets/World Area Grid.xlsx
+++ b/Cuisine Quest/Assets/World Area Grid.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\johnc\Documents\GitHub\Cuisine-Quest\Cuisine Quest\Assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14DBC0B-9697-4FDD-B72C-04445265B8A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26819"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C56D70ED-9BC3-480F-8831-0A60697E4425}"/>
+    <workbookView xWindow="1720" yWindow="280" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -222,7 +219,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -232,12 +229,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -252,8 +255,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,7 +318,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -366,7 +370,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -560,27 +564,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC01B993-962A-498A-838D-8251CED4F6E8}">
-  <dimension ref="A1:F37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,403 +604,423 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>-48</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>-48</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>10</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
         <v>-3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>-48</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>20</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>-48</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>30</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>4.5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>-1.5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>-48</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>40</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>4.5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>-32</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>40</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1.5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>-3</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>-32</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>30</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>1.5</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>-1.5</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>-32</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>20</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>1.5</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>-32</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>10</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>-32</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
         <v>-6</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>3.5</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13">
+      <c r="B12" s="1">
         <v>-16</v>
       </c>
-      <c r="C13">
+      <c r="C12" s="1">
         <v>30</v>
       </c>
-      <c r="F13" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14">
+      <c r="B13" s="1">
         <v>-16</v>
       </c>
-      <c r="C14">
+      <c r="C13" s="1">
         <v>20</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F13" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15">
+      <c r="B14" s="1">
         <v>-16</v>
       </c>
-      <c r="C15">
+      <c r="C14" s="1">
         <v>10</v>
       </c>
-      <c r="D15">
+      <c r="D14" s="1">
         <v>4.5</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B16">
+      <c r="B15" s="1">
         <v>-16</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <v>3.5</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F15" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
         <v>20</v>
       </c>
-      <c r="D17">
+      <c r="D16" s="1">
         <v>-2.5</v>
       </c>
-      <c r="E17">
+      <c r="E16" s="1">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F16" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
         <v>10</v>
       </c>
-      <c r="D18">
+      <c r="D17" s="1">
         <v>-2.5</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
         <v>-3</v>
       </c>
-      <c r="E19">
+      <c r="E18" s="1">
         <v>3</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F18" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B20">
+      <c r="B19" s="1">
         <v>16</v>
       </c>
-      <c r="C20">
+      <c r="C19" s="1">
         <v>20</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F19" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21">
-        <v>-3</v>
+        <v>-19</v>
       </c>
       <c r="C21">
         <v>-4</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>-19</v>
       </c>
       <c r="C22">
-        <v>-4</v>
+        <v>-14</v>
       </c>
       <c r="D22">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>-19</v>
       </c>
       <c r="C23">
-        <v>-14</v>
+        <v>-24</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1005,12 +1029,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24">
-        <v>-19</v>
+        <v>-35</v>
       </c>
       <c r="C24">
         <v>-24</v>
@@ -1022,15 +1046,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>-35</v>
       </c>
       <c r="C25">
-        <v>-24</v>
+        <v>-14</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1039,136 +1063,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>-35</v>
       </c>
       <c r="C26">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>-3</v>
+      </c>
+      <c r="C27">
         <v>-14</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27">
-        <v>-35</v>
-      </c>
-      <c r="C27">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>-3</v>
       </c>
       <c r="C28">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29">
-        <v>-3</v>
-      </c>
-      <c r="C29">
         <v>-24</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="1">
+        <v>-80</v>
+      </c>
+      <c r="C29" s="1">
+        <v>20</v>
+      </c>
+      <c r="D29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30">
-        <v>-80</v>
-      </c>
-      <c r="C30">
-        <v>20</v>
-      </c>
-      <c r="D30">
-        <v>-1</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="1">
+        <v>16</v>
+      </c>
+      <c r="C31" s="1">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E31" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37">
-        <v>16</v>
-      </c>
-      <c r="C37">
-        <v>30</v>
-      </c>
-      <c r="D37">
-        <v>0.5</v>
-      </c>
-      <c r="E37">
-        <v>-0.5</v>
-      </c>
-      <c r="F37" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>